<commit_message>
removed src. from imports
</commit_message>
<xml_diff>
--- a/src/stats.xlsx
+++ b/src/stats.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Depth = 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth = 7</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Depth = 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth = 5</t>
   </si>
   <si>
     <t xml:space="preserve">CoinParity</t>
@@ -46,10 +46,43 @@
     <t xml:space="preserve">Mobility + ab</t>
   </si>
   <si>
-    <t xml:space="preserve">Depth=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth=7</t>
+    <t xml:space="preserve">Depth=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8|0|17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16|0|9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7|2|16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12|0|13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7|1|17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">defeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time [s]</t>
   </si>
 </sst>
 </file>
@@ -59,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -80,13 +113,29 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -130,7 +179,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -147,6 +196,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,7 +213,367 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Average Game Length </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>935</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3298</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="85004798"/>
+        <c:axId val="16692176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="85004798"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16692176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="16692176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Time [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85004798"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>769680</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>112320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>26640</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>100800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="9028800" y="4013640"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -164,10 +581,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:N26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -245,7 +662,9 @@
         <f aca="false">C$4</f>
         <v>CoinParity</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -263,7 +682,9 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -281,7 +702,9 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -299,7 +722,9 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -315,9 +740,11 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -335,7 +762,9 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -350,7 +779,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="str">
         <f aca="false">C$4</f>
@@ -408,7 +837,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -458,6 +887,89 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>24.9</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>935</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>3298</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -473,5 +985,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
search function returns value on only one place
</commit_message>
<xml_diff>
--- a/src/stats.xlsx
+++ b/src/stats.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
-  <si>
-    <t xml:space="preserve">Depth = 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth = 5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">D=5</t>
   </si>
   <si>
     <t xml:space="preserve">CoinParity</t>
@@ -37,18 +34,6 @@
     <t xml:space="preserve">Mobility</t>
   </si>
   <si>
-    <t xml:space="preserve">CoinParity + ab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weights + ab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobility + ab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth=3</t>
-  </si>
-  <si>
     <t xml:space="preserve">8|0|17</t>
   </si>
   <si>
@@ -56,15 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">7|2|16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12|0|13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7|1|17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth=5</t>
   </si>
   <si>
     <t xml:space="preserve">win</t>
@@ -92,11 +68,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -115,6 +92,11 @@
     </font>
     <font>
       <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -179,20 +161,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,7 +262,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -328,6 +314,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -339,6 +326,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -383,11 +371,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="85004798"/>
-        <c:axId val="16692176"/>
+        <c:axId val="20917739"/>
+        <c:axId val="91686497"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85004798"/>
+        <c:axId val="20917739"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,14 +431,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16692176"/>
+        <c:crossAx val="91686497"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16692176"/>
+        <c:axId val="91686497"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -493,7 +481,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -515,7 +503,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85004798"/>
+        <c:crossAx val="20917739"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -534,7 +522,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -552,9 +540,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>26640</xdr:colOff>
+      <xdr:colOff>26280</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -562,8 +550,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9028800" y="4013640"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="9035280" y="4013640"/>
+        <a:ext cx="5769000" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -584,10 +572,10 @@
   <dimension ref="A3:N26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.03"/>
@@ -597,17 +585,15 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -616,57 +602,37 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="str">
         <f aca="false">C$4</f>
         <v>CoinParity</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -678,15 +644,17 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -698,15 +666,15 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -718,13 +686,9 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -738,13 +702,9 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -758,13 +718,9 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -778,13 +734,8 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="str">
-        <f aca="false">C$4</f>
-        <v>CoinParity</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -799,10 +750,8 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -817,10 +766,8 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -835,10 +782,8 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -853,10 +798,8 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -871,10 +814,8 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -890,18 +831,18 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>25</v>
@@ -915,7 +856,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1</v>
@@ -943,8 +884,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
+      <c r="A26" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.8</v>
@@ -972,12 +913,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A16"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Square attribute occupied is now a method
</commit_message>
<xml_diff>
--- a/src/stats.xlsx
+++ b/src/stats.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t xml:space="preserve">D=5</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">8|0|17</t>
   </si>
   <si>
+    <t xml:space="preserve">12|1|12</t>
+  </si>
+  <si>
     <t xml:space="preserve">16|0|9</t>
   </si>
   <si>
@@ -59,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">Time [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1vs5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5|1|19</t>
   </si>
 </sst>
 </file>
@@ -262,7 +271,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -371,11 +380,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="20917739"/>
-        <c:axId val="91686497"/>
+        <c:axId val="29787982"/>
+        <c:axId val="6660726"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="20917739"/>
+        <c:axId val="29787982"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,14 +440,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91686497"/>
+        <c:crossAx val="6660726"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91686497"/>
+        <c:axId val="6660726"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,7 +512,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20917739"/>
+        <c:crossAx val="29787982"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -569,10 +578,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:N26"/>
+  <dimension ref="A3:N30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -631,7 +640,9 @@
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -651,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -671,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -831,18 +842,18 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>25</v>
@@ -856,7 +867,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1</v>
@@ -885,7 +896,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.8</v>
@@ -910,6 +921,19 @@
       </c>
       <c r="I26" s="0" t="n">
         <v>3298</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>